<commit_message>
Updated codes with alert
</commit_message>
<xml_diff>
--- a/com.demoAutomationsite/TestData/Demosite.xlsx
+++ b/com.demoAutomationsite/TestData/Demosite.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="8">
   <si>
     <t xml:space="preserve">john </t>
   </si>
@@ -33,13 +33,19 @@
     <t xml:space="preserve">Amul@mailinator.com</t>
   </si>
   <si>
-    <t xml:space="preserve">batista</t>
-  </si>
-  <si>
-    <t xml:space="preserve">animal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gow@mailinator.com</t>
+    <t xml:space="preserve">arnolf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g2@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gm@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gh@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -137,16 +143,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.75"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -159,7 +162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
@@ -170,11 +173,122 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C1" r:id="rId1" display="Amul@mailinator.com"/>
-    <hyperlink ref="C2" r:id="rId2" display="gow@mailinator.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="g2@mailinator.com"/>
+    <hyperlink ref="C3" r:id="rId3" display="gm@mailinator.com"/>
+    <hyperlink ref="C4" r:id="rId4" display="gh@mailinator.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -198,9 +312,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.75"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -224,9 +335,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.75"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>